<commit_message>
Update file generated from new code
</commit_message>
<xml_diff>
--- a/ACHM_FC_comparison.xlsx
+++ b/ACHM_FC_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\keeran\map-synchronization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83E0DF9-5B1D-4A0E-9DB6-B65C65CBF7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049CE080-49FA-4D44-BCF2-68FB8ABC79AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="10080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="10710" windowWidth="29040" windowHeight="17025" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Present in all maps" sheetId="1" r:id="rId1"/>
@@ -1519,7 +1519,7 @@
     <t>reproductive_13-1</t>
   </si>
   <si>
-    <t>Not in FC</t>
+    <t>NOT IN FC</t>
   </si>
   <si>
     <t>Acetylcholine (muscarinic) receptor</t>
@@ -4159,7 +4159,7 @@
     <t>digestive_60-1</t>
   </si>
   <si>
-    <t>Not in AC Human Male</t>
+    <t>NOT IN AC HUMAN MALE</t>
   </si>
   <si>
     <t>ILX:0001473</t>
@@ -9950,20 +9950,36 @@
     <t>organ-blocks/slide-01/6606</t>
   </si>
   <si>
-    <t>Need to add to FC</t>
-  </si>
-  <si>
-    <t>Need to add to AC Human Male</t>
+    <t>NEED TO ADD TO FC</t>
+  </si>
+  <si>
+    <t>NEED TO ADD TO AC HUMAN MALE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9989,8 +10005,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10331,23 +10349,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="74.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.68359375" customWidth="1"/>
+    <col min="2" max="3" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -12179,22 +12196,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="72.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.68359375" customWidth="1"/>
+    <col min="2" max="2" width="35.68359375" customWidth="1"/>
+    <col min="3" max="4" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15434,23 +15451,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.68359375" customWidth="1"/>
+    <col min="2" max="2" width="35.68359375" customWidth="1"/>
+    <col min="3" max="4" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1378</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -22500,43 +22516,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H641"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.41796875" customWidth="1"/>
+    <col min="1" max="1" width="19.47265625" customWidth="1"/>
+    <col min="2" max="2" width="30.68359375" customWidth="1"/>
     <col min="3" max="3" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.62890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.9453125" customWidth="1"/>
-    <col min="7" max="7" width="34.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.734375" customWidth="1"/>
+    <col min="5" max="5" width="30.68359375" customWidth="1"/>
+    <col min="6" max="6" width="35.68359375" customWidth="1"/>
+    <col min="7" max="7" width="15.68359375" customWidth="1"/>
     <col min="8" max="8" width="30.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3298</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3299</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>